<commit_message>
Added HD_Drive_Stops.xml and C27876-X_HD Prec Angle Adj.xml to ERP Model28.xlsx and Safety Whl Ass'y_8026015-X.xlsx were touched to update their hash because their contents were already added but still being listed as dirty.
</commit_message>
<xml_diff>
--- a/OpsAndMats/Model28.xlsx
+++ b/OpsAndMats/Model28.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eclark.LABTESTING\Documents\ERP Notes\Phase2_BOM\OpsAndMats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD49699-689D-4F34-BDAF-1EFC2B5AA043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CA9A1A-DB7B-4C5F-8C30-CF26CD5321AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>